<commit_message>
Feat: Add two sections
</commit_message>
<xml_diff>
--- a/Dados BMS/Lista_Pontos_Chiller.xlsx
+++ b/Dados BMS/Lista_Pontos_Chiller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cveigam\00 Projects\04_TCC_AED\USP_TCC_ML_CHILLER\Dados BMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F487DC-DB15-41F9-B42F-0F1EB8A11C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAFADAD-D175-431B-BC31-13515860BFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15405" yWindow="2910" windowWidth="29040" windowHeight="15990" xr2:uid="{65A5F944-6BC8-42A4-93EA-278606816E42}"/>
   </bookViews>
@@ -36,26 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>PointName</t>
   </si>
   <si>
-    <t>Tipo equipamento</t>
-  </si>
-  <si>
-    <t>Nome equipamento</t>
-  </si>
-  <si>
     <t>Ponto</t>
   </si>
   <si>
     <t>S1-ADX1:S1-ADX-NAE1/S1-ADX1-NAE1-TR1.Chiller 2.Analog Values.AV-6.Present Value</t>
   </si>
   <si>
-    <t>Chiller</t>
-  </si>
-  <si>
     <t>ur_temp_entrada</t>
   </si>
   <si>
@@ -95,10 +86,16 @@
     <t>ur_correnteMotor</t>
   </si>
   <si>
-    <t>S1-ADX1:S1-ADX-NAE4/S1-ADX1-NAE4-TR1.QAC-6PV-03-B.TC-06-03.TC-06-03 - STE.Present Value</t>
-  </si>
-  <si>
-    <t>temp_externa</t>
+    <t>S1-ADX1:S1-ADX-NAE1/S1-ADX1-NAE1-TR1.FAC QAC-CAG-01.SPD-MIN.Present Value</t>
+  </si>
+  <si>
+    <t>Pressao_PR_min</t>
+  </si>
+  <si>
+    <t>Equipamento</t>
+  </si>
+  <si>
+    <t>Chiller 2</t>
   </si>
 </sst>
 </file>
@@ -114,9 +111,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,9 +137,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,144 +473,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552C512C-D9D5-4839-B97B-386A346B819A}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="86.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="86.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>